<commit_message>
Update TimeOFF testcases and made it as data driven
</commit_message>
<xml_diff>
--- a/Data/LeaveRequest.xlsx
+++ b/Data/LeaveRequest.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7147B87A-2205-43AE-8433-0EA6B8E32A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
   </numFmts>
@@ -126,42 +127,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -479,21 +445,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="7" max="8" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" customWidth="1"/>
+    <col min="7" max="8" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +489,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>10648866</v>
       </c>
@@ -551,7 +518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>10648866</v>
       </c>
@@ -582,28 +549,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1 E3">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>